<commit_message>
Tối ưu thuật toán GA - Giải quyết xung đột phát sinh sau khi tạo lịch
</commit_message>
<xml_diff>
--- a/timetabling_GA/results/HK1_CT03/TKB_HocKy_GiangVien.xlsx
+++ b/timetabling_GA/results/HK1_CT03/TKB_HocKy_GiangVien.xlsx
@@ -506,7 +506,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -598,8 +598,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>S1
-(07:00-09:00)</t>
+          <t>S2
+(09:00-11:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -608,24 +608,31 @@
         </is>
       </c>
       <c r="C8" s="7" t="inlineStr"/>
-      <c r="D8" s="8" t="inlineStr">
+      <c r="D8" s="7" t="inlineStr"/>
+      <c r="E8" s="7" t="inlineStr"/>
+      <c r="F8" s="7" t="inlineStr"/>
+      <c r="G8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Tiếng Anh chuyên ngành
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H8" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
 Môn: Tiếng Anh chuyên ngành
-Phòng: R101
-(Lý thuyết)</t>
-        </is>
-      </c>
-      <c r="E8" s="7" t="inlineStr"/>
-      <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="7" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
+Phòng: R105
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C2
-(15:00-17:00)</t>
+          <t>C1
+(13:00-15:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -636,16 +643,42 @@
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
       <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="8" t="inlineStr">
+      <c r="F9" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
 Môn: Kỹ năng mềm
-Phòng: R101
-(Lý thuyết)</t>
-        </is>
-      </c>
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
+    </row>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>T1
+(17:30-19:30)</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>Ngô Văn I</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="inlineStr"/>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="7" t="inlineStr"/>
+      <c r="G10" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Kỹ năng mềm
+Phòng: R104
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H10" s="7" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -664,7 +697,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -756,8 +789,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>S1
-(07:00-09:00)</t>
+          <t>S2
+(09:00-11:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -766,24 +799,31 @@
         </is>
       </c>
       <c r="C8" s="7" t="inlineStr"/>
-      <c r="D8" s="8" t="inlineStr">
+      <c r="D8" s="7" t="inlineStr"/>
+      <c r="E8" s="7" t="inlineStr"/>
+      <c r="F8" s="7" t="inlineStr"/>
+      <c r="G8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Tiếng Anh chuyên ngành
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H8" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
 Môn: Tiếng Anh chuyên ngành
-Phòng: R101
-(Lý thuyết)</t>
-        </is>
-      </c>
-      <c r="E8" s="7" t="inlineStr"/>
-      <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="7" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
+Phòng: R105
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C2
-(15:00-17:00)</t>
+          <t>C1
+(13:00-15:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -794,16 +834,42 @@
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
       <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="8" t="inlineStr">
+      <c r="F9" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
 Môn: Kỹ năng mềm
-Phòng: R101
-(Lý thuyết)</t>
-        </is>
-      </c>
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
+    </row>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>T1
+(17:30-19:30)</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>Ngô Văn I</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="inlineStr"/>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="7" t="inlineStr"/>
+      <c r="G10" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Kỹ năng mềm
+Phòng: R104
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H10" s="7" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -822,7 +888,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -914,8 +980,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>S1
-(07:00-09:00)</t>
+          <t>S2
+(09:00-11:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -924,24 +990,31 @@
         </is>
       </c>
       <c r="C8" s="7" t="inlineStr"/>
-      <c r="D8" s="8" t="inlineStr">
+      <c r="D8" s="7" t="inlineStr"/>
+      <c r="E8" s="7" t="inlineStr"/>
+      <c r="F8" s="7" t="inlineStr"/>
+      <c r="G8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Tiếng Anh chuyên ngành
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H8" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
 Môn: Tiếng Anh chuyên ngành
-Phòng: R101
-(Lý thuyết)</t>
-        </is>
-      </c>
-      <c r="E8" s="7" t="inlineStr"/>
-      <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="7" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
+Phòng: R105
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C2
-(15:00-17:00)</t>
+          <t>C1
+(13:00-15:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -952,16 +1025,42 @@
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
       <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="8" t="inlineStr">
+      <c r="F9" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
 Môn: Kỹ năng mềm
-Phòng: R101
-(Lý thuyết)</t>
-        </is>
-      </c>
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
+    </row>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>T1
+(17:30-19:30)</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>Ngô Văn I</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="inlineStr"/>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="7" t="inlineStr"/>
+      <c r="G10" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Kỹ năng mềm
+Phòng: R104
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H10" s="7" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -980,7 +1079,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1072,8 +1171,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>S1
-(07:00-09:00)</t>
+          <t>S2
+(09:00-11:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -1082,24 +1181,31 @@
         </is>
       </c>
       <c r="C8" s="7" t="inlineStr"/>
-      <c r="D8" s="8" t="inlineStr">
+      <c r="D8" s="7" t="inlineStr"/>
+      <c r="E8" s="7" t="inlineStr"/>
+      <c r="F8" s="7" t="inlineStr"/>
+      <c r="G8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Tiếng Anh chuyên ngành
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H8" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
 Môn: Tiếng Anh chuyên ngành
-Phòng: R101
-(Lý thuyết)</t>
-        </is>
-      </c>
-      <c r="E8" s="7" t="inlineStr"/>
-      <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="7" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
+Phòng: R105
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C2
-(15:00-17:00)</t>
+          <t>C1
+(13:00-15:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -1110,16 +1216,42 @@
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
       <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="8" t="inlineStr">
+      <c r="F9" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
 Môn: Kỹ năng mềm
-Phòng: R101
-(Lý thuyết)</t>
-        </is>
-      </c>
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
+    </row>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>T1
+(17:30-19:30)</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>Ngô Văn I</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="inlineStr"/>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="7" t="inlineStr"/>
+      <c r="G10" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Kỹ năng mềm
+Phòng: R104
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H10" s="7" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1138,7 +1270,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1230,8 +1362,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>S1
-(07:00-09:00)</t>
+          <t>S2
+(09:00-11:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -1240,24 +1372,31 @@
         </is>
       </c>
       <c r="C8" s="7" t="inlineStr"/>
-      <c r="D8" s="8" t="inlineStr">
+      <c r="D8" s="7" t="inlineStr"/>
+      <c r="E8" s="7" t="inlineStr"/>
+      <c r="F8" s="7" t="inlineStr"/>
+      <c r="G8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Tiếng Anh chuyên ngành
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H8" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
 Môn: Tiếng Anh chuyên ngành
-Phòng: R101
-(Lý thuyết)</t>
-        </is>
-      </c>
-      <c r="E8" s="7" t="inlineStr"/>
-      <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="7" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
+Phòng: R105
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C2
-(15:00-17:00)</t>
+          <t>C1
+(13:00-15:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -1268,16 +1407,42 @@
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
       <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="8" t="inlineStr">
+      <c r="F9" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
 Môn: Kỹ năng mềm
-Phòng: R101
-(Lý thuyết)</t>
-        </is>
-      </c>
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
+    </row>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>T1
+(17:30-19:30)</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>Ngô Văn I</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="inlineStr"/>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="7" t="inlineStr"/>
+      <c r="G10" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Kỹ năng mềm
+Phòng: R104
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H10" s="7" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1296,7 +1461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1388,8 +1553,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>S1
-(07:00-09:00)</t>
+          <t>S2
+(09:00-11:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -1398,24 +1563,31 @@
         </is>
       </c>
       <c r="C8" s="7" t="inlineStr"/>
-      <c r="D8" s="8" t="inlineStr">
+      <c r="D8" s="7" t="inlineStr"/>
+      <c r="E8" s="7" t="inlineStr"/>
+      <c r="F8" s="7" t="inlineStr"/>
+      <c r="G8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Tiếng Anh chuyên ngành
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H8" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
 Môn: Tiếng Anh chuyên ngành
-Phòng: R101
-(Lý thuyết)</t>
-        </is>
-      </c>
-      <c r="E8" s="7" t="inlineStr"/>
-      <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="7" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
+Phòng: R105
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C2
-(15:00-17:00)</t>
+          <t>C1
+(13:00-15:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -1426,16 +1598,42 @@
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
       <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="8" t="inlineStr">
+      <c r="F9" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
 Môn: Kỹ năng mềm
-Phòng: R101
-(Lý thuyết)</t>
-        </is>
-      </c>
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
+    </row>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>T1
+(17:30-19:30)</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>Ngô Văn I</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="inlineStr"/>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="7" t="inlineStr"/>
+      <c r="G10" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Kỹ năng mềm
+Phòng: R104
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H10" s="7" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1454,7 +1652,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1546,8 +1744,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>S1
-(07:00-09:00)</t>
+          <t>S2
+(09:00-11:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -1556,24 +1754,31 @@
         </is>
       </c>
       <c r="C8" s="7" t="inlineStr"/>
-      <c r="D8" s="8" t="inlineStr">
+      <c r="D8" s="7" t="inlineStr"/>
+      <c r="E8" s="7" t="inlineStr"/>
+      <c r="F8" s="7" t="inlineStr"/>
+      <c r="G8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Tiếng Anh chuyên ngành
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H8" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
 Môn: Tiếng Anh chuyên ngành
-Phòng: R101
-(Lý thuyết)</t>
-        </is>
-      </c>
-      <c r="E8" s="7" t="inlineStr"/>
-      <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="7" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
+Phòng: R105
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C2
-(15:00-17:00)</t>
+          <t>C1
+(13:00-15:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -1584,16 +1789,42 @@
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
       <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="8" t="inlineStr">
+      <c r="F9" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
 Môn: Kỹ năng mềm
-Phòng: R101
-(Lý thuyết)</t>
-        </is>
-      </c>
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
+    </row>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>T1
+(17:30-19:30)</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>Ngô Văn I</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="inlineStr"/>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="7" t="inlineStr"/>
+      <c r="G10" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Kỹ năng mềm
+Phòng: R104
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H10" s="7" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1612,7 +1843,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1704,8 +1935,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>S1
-(07:00-09:00)</t>
+          <t>S2
+(09:00-11:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -1714,24 +1945,31 @@
         </is>
       </c>
       <c r="C8" s="7" t="inlineStr"/>
-      <c r="D8" s="8" t="inlineStr">
+      <c r="D8" s="7" t="inlineStr"/>
+      <c r="E8" s="7" t="inlineStr"/>
+      <c r="F8" s="7" t="inlineStr"/>
+      <c r="G8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Tiếng Anh chuyên ngành
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H8" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
 Môn: Tiếng Anh chuyên ngành
-Phòng: R101
-(Lý thuyết)</t>
-        </is>
-      </c>
-      <c r="E8" s="7" t="inlineStr"/>
-      <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="7" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
+Phòng: R105
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C2
-(15:00-17:00)</t>
+          <t>C1
+(13:00-15:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -1742,16 +1980,42 @@
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
       <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="8" t="inlineStr">
+      <c r="F9" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
 Môn: Kỹ năng mềm
-Phòng: R101
-(Lý thuyết)</t>
-        </is>
-      </c>
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
+    </row>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>T1
+(17:30-19:30)</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>Ngô Văn I</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="inlineStr"/>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="7" t="inlineStr"/>
+      <c r="G10" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Kỹ năng mềm
+Phòng: R104
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H10" s="7" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1770,7 +2034,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1862,8 +2126,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>S1
-(07:00-09:00)</t>
+          <t>S2
+(09:00-11:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -1872,24 +2136,31 @@
         </is>
       </c>
       <c r="C8" s="7" t="inlineStr"/>
-      <c r="D8" s="8" t="inlineStr">
+      <c r="D8" s="7" t="inlineStr"/>
+      <c r="E8" s="7" t="inlineStr"/>
+      <c r="F8" s="7" t="inlineStr"/>
+      <c r="G8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Tiếng Anh chuyên ngành
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H8" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
 Môn: Tiếng Anh chuyên ngành
-Phòng: R101
-(Lý thuyết)</t>
-        </is>
-      </c>
-      <c r="E8" s="7" t="inlineStr"/>
-      <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="7" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
+Phòng: R105
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C2
-(15:00-17:00)</t>
+          <t>C1
+(13:00-15:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -1900,16 +2171,42 @@
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
       <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="8" t="inlineStr">
+      <c r="F9" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
 Môn: Kỹ năng mềm
-Phòng: R101
-(Lý thuyết)</t>
-        </is>
-      </c>
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
+    </row>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>T1
+(17:30-19:30)</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>Ngô Văn I</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="inlineStr"/>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="7" t="inlineStr"/>
+      <c r="G10" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Kỹ năng mềm
+Phòng: R104
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H10" s="7" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1928,7 +2225,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2020,8 +2317,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>S1
-(07:00-09:00)</t>
+          <t>S2
+(09:00-11:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -2030,24 +2327,31 @@
         </is>
       </c>
       <c r="C8" s="7" t="inlineStr"/>
-      <c r="D8" s="8" t="inlineStr">
+      <c r="D8" s="7" t="inlineStr"/>
+      <c r="E8" s="7" t="inlineStr"/>
+      <c r="F8" s="7" t="inlineStr"/>
+      <c r="G8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Tiếng Anh chuyên ngành
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H8" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
 Môn: Tiếng Anh chuyên ngành
-Phòng: R101
-(Lý thuyết)</t>
-        </is>
-      </c>
-      <c r="E8" s="7" t="inlineStr"/>
-      <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="7" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
+Phòng: R105
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C2
-(15:00-17:00)</t>
+          <t>C1
+(13:00-15:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -2058,16 +2362,42 @@
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
       <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="8" t="inlineStr">
+      <c r="F9" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
 Môn: Kỹ năng mềm
-Phòng: R101
-(Lý thuyết)</t>
-        </is>
-      </c>
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
+    </row>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>T1
+(17:30-19:30)</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>Ngô Văn I</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="inlineStr"/>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="7" t="inlineStr"/>
+      <c r="G10" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Kỹ năng mềm
+Phòng: R104
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H10" s="7" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2086,7 +2416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2178,8 +2508,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>S1
-(07:00-09:00)</t>
+          <t>S2
+(09:00-11:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -2188,24 +2518,31 @@
         </is>
       </c>
       <c r="C8" s="7" t="inlineStr"/>
-      <c r="D8" s="8" t="inlineStr">
+      <c r="D8" s="7" t="inlineStr"/>
+      <c r="E8" s="7" t="inlineStr"/>
+      <c r="F8" s="7" t="inlineStr"/>
+      <c r="G8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Tiếng Anh chuyên ngành
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H8" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
 Môn: Tiếng Anh chuyên ngành
-Phòng: R101
-(Lý thuyết)</t>
-        </is>
-      </c>
-      <c r="E8" s="7" t="inlineStr"/>
-      <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="7" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
+Phòng: R105
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C2
-(15:00-17:00)</t>
+          <t>C1
+(13:00-15:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -2216,16 +2553,42 @@
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
       <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="8" t="inlineStr">
+      <c r="F9" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
 Môn: Kỹ năng mềm
-Phòng: R101
-(Lý thuyết)</t>
-        </is>
-      </c>
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
+    </row>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>T1
+(17:30-19:30)</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>Ngô Văn I</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="inlineStr"/>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="7" t="inlineStr"/>
+      <c r="G10" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Kỹ năng mềm
+Phòng: R104
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H10" s="7" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2244,7 +2607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2336,8 +2699,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>S1
-(07:00-09:00)</t>
+          <t>S2
+(09:00-11:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -2346,24 +2709,31 @@
         </is>
       </c>
       <c r="C8" s="7" t="inlineStr"/>
-      <c r="D8" s="8" t="inlineStr">
+      <c r="D8" s="7" t="inlineStr"/>
+      <c r="E8" s="7" t="inlineStr"/>
+      <c r="F8" s="7" t="inlineStr"/>
+      <c r="G8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Tiếng Anh chuyên ngành
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H8" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
 Môn: Tiếng Anh chuyên ngành
-Phòng: R101
-(Lý thuyết)</t>
-        </is>
-      </c>
-      <c r="E8" s="7" t="inlineStr"/>
-      <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="7" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
+Phòng: R105
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C2
-(15:00-17:00)</t>
+          <t>C1
+(13:00-15:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -2374,16 +2744,42 @@
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
       <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="8" t="inlineStr">
+      <c r="F9" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
 Môn: Kỹ năng mềm
-Phòng: R101
-(Lý thuyết)</t>
-        </is>
-      </c>
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
+    </row>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>T1
+(17:30-19:30)</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>Ngô Văn I</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="inlineStr"/>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="7" t="inlineStr"/>
+      <c r="G10" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Kỹ năng mềm
+Phòng: R104
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H10" s="7" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2402,7 +2798,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2494,8 +2890,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>S1
-(07:00-09:00)</t>
+          <t>S2
+(09:00-11:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -2504,24 +2900,31 @@
         </is>
       </c>
       <c r="C8" s="7" t="inlineStr"/>
-      <c r="D8" s="8" t="inlineStr">
+      <c r="D8" s="7" t="inlineStr"/>
+      <c r="E8" s="7" t="inlineStr"/>
+      <c r="F8" s="7" t="inlineStr"/>
+      <c r="G8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Tiếng Anh chuyên ngành
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H8" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
 Môn: Tiếng Anh chuyên ngành
-Phòng: R101
-(Lý thuyết)</t>
-        </is>
-      </c>
-      <c r="E8" s="7" t="inlineStr"/>
-      <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="7" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
+Phòng: R105
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C2
-(15:00-17:00)</t>
+          <t>C1
+(13:00-15:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -2532,16 +2935,42 @@
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
       <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="8" t="inlineStr">
+      <c r="F9" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
 Môn: Kỹ năng mềm
-Phòng: R101
-(Lý thuyết)</t>
-        </is>
-      </c>
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
+    </row>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>T1
+(17:30-19:30)</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>Ngô Văn I</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="inlineStr"/>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="7" t="inlineStr"/>
+      <c r="G10" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Kỹ năng mềm
+Phòng: R104
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H10" s="7" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2560,7 +2989,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2652,8 +3081,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>S1
-(07:00-09:00)</t>
+          <t>S2
+(09:00-11:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -2662,24 +3091,31 @@
         </is>
       </c>
       <c r="C8" s="7" t="inlineStr"/>
-      <c r="D8" s="8" t="inlineStr">
+      <c r="D8" s="7" t="inlineStr"/>
+      <c r="E8" s="7" t="inlineStr"/>
+      <c r="F8" s="7" t="inlineStr"/>
+      <c r="G8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Tiếng Anh chuyên ngành
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H8" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
 Môn: Tiếng Anh chuyên ngành
-Phòng: R101
-(Lý thuyết)</t>
-        </is>
-      </c>
-      <c r="E8" s="7" t="inlineStr"/>
-      <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="7" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
+Phòng: R105
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C2
-(15:00-17:00)</t>
+          <t>C1
+(13:00-15:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -2690,16 +3126,42 @@
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
       <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="8" t="inlineStr">
+      <c r="F9" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
 Môn: Kỹ năng mềm
-Phòng: R101
-(Lý thuyết)</t>
-        </is>
-      </c>
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
+    </row>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>T1
+(17:30-19:30)</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>Ngô Văn I</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="inlineStr"/>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="7" t="inlineStr"/>
+      <c r="G10" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Kỹ năng mềm
+Phòng: R104
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H10" s="7" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2718,7 +3180,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2810,8 +3272,8 @@
     <row r="8" ht="60" customHeight="1">
       <c r="A8" s="6" t="inlineStr">
         <is>
-          <t>S1
-(07:00-09:00)</t>
+          <t>S2
+(09:00-11:00)</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
@@ -2820,24 +3282,31 @@
         </is>
       </c>
       <c r="C8" s="7" t="inlineStr"/>
-      <c r="D8" s="8" t="inlineStr">
+      <c r="D8" s="7" t="inlineStr"/>
+      <c r="E8" s="7" t="inlineStr"/>
+      <c r="F8" s="7" t="inlineStr"/>
+      <c r="G8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Tiếng Anh chuyên ngành
+Phòng: R102
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H8" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
 Môn: Tiếng Anh chuyên ngành
-Phòng: R101
-(Lý thuyết)</t>
-        </is>
-      </c>
-      <c r="E8" s="7" t="inlineStr"/>
-      <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="7" t="inlineStr"/>
-      <c r="H8" s="7" t="inlineStr"/>
+Phòng: R105
+(Lý thuyết)</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C2
-(15:00-17:00)</t>
+          <t>C1
+(13:00-15:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -2848,16 +3317,42 @@
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
       <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="7" t="inlineStr"/>
-      <c r="G9" s="8" t="inlineStr">
+      <c r="F9" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
 Môn: Kỹ năng mềm
-Phòng: R101
-(Lý thuyết)</t>
-        </is>
-      </c>
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
+    </row>
+    <row r="10" ht="60" customHeight="1">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>T1
+(17:30-19:30)</t>
+        </is>
+      </c>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>Ngô Văn I</t>
+        </is>
+      </c>
+      <c r="C10" s="7" t="inlineStr"/>
+      <c r="D10" s="7" t="inlineStr"/>
+      <c r="E10" s="7" t="inlineStr"/>
+      <c r="F10" s="7" t="inlineStr"/>
+      <c r="G10" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Kỹ năng mềm
+Phòng: R104
+(Lý thuyết)</t>
+        </is>
+      </c>
+      <c r="H10" s="7" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Cải tiến thuật toán GA - Xử lý xung đột theo tuần
</commit_message>
<xml_diff>
--- a/timetabling_GA/results/HK1_CT03/TKB_HocKy_GiangVien.xlsx
+++ b/timetabling_GA/results/HK1_CT03/TKB_HocKy_GiangVien.xlsx
@@ -604,21 +604,21 @@
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>Võ Văn F</t>
+          <t>Hoàng Thị E</t>
         </is>
       </c>
       <c r="C8" s="7" t="inlineStr"/>
-      <c r="D8" s="7" t="inlineStr"/>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL05
+Môn: Kỹ năng mềm
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL10
-Môn: Tiếng Anh chuyên ngành
-Phòng: R102
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
@@ -631,8 +631,8 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C1
-(13:00-15:00)</t>
+          <t>C2
+(15:00-17:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -643,15 +643,15 @@
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
       <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL05
-Môn: Kỹ năng mềm
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Tiếng Anh chuyên ngành
 Phòng: R103
 (Lý thuyết)</t>
         </is>
       </c>
-      <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
     </row>
     <row r="10" ht="60" customHeight="1">
@@ -663,7 +663,7 @@
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>Ngô Văn I</t>
+          <t>Hoàng Thị E</t>
         </is>
       </c>
       <c r="C10" s="7" t="inlineStr"/>
@@ -674,7 +674,7 @@
         <is>
           <t>Lớp: CL10
 Môn: Kỹ năng mềm
-Phòng: R104
+Phòng: R101
 (Lý thuyết)</t>
         </is>
       </c>
@@ -795,21 +795,21 @@
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>Võ Văn F</t>
+          <t>Hoàng Thị E</t>
         </is>
       </c>
       <c r="C8" s="7" t="inlineStr"/>
-      <c r="D8" s="7" t="inlineStr"/>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL05
+Môn: Kỹ năng mềm
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL10
-Môn: Tiếng Anh chuyên ngành
-Phòng: R102
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
@@ -822,8 +822,8 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C1
-(13:00-15:00)</t>
+          <t>C2
+(15:00-17:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -834,15 +834,15 @@
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
       <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL05
-Môn: Kỹ năng mềm
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Tiếng Anh chuyên ngành
 Phòng: R103
 (Lý thuyết)</t>
         </is>
       </c>
-      <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
     </row>
     <row r="10" ht="60" customHeight="1">
@@ -854,7 +854,7 @@
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>Ngô Văn I</t>
+          <t>Hoàng Thị E</t>
         </is>
       </c>
       <c r="C10" s="7" t="inlineStr"/>
@@ -865,7 +865,7 @@
         <is>
           <t>Lớp: CL10
 Môn: Kỹ năng mềm
-Phòng: R104
+Phòng: R101
 (Lý thuyết)</t>
         </is>
       </c>
@@ -986,21 +986,21 @@
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>Võ Văn F</t>
+          <t>Hoàng Thị E</t>
         </is>
       </c>
       <c r="C8" s="7" t="inlineStr"/>
-      <c r="D8" s="7" t="inlineStr"/>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL05
+Môn: Kỹ năng mềm
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL10
-Môn: Tiếng Anh chuyên ngành
-Phòng: R102
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
@@ -1013,8 +1013,8 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C1
-(13:00-15:00)</t>
+          <t>C2
+(15:00-17:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -1025,15 +1025,15 @@
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
       <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL05
-Môn: Kỹ năng mềm
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Tiếng Anh chuyên ngành
 Phòng: R103
 (Lý thuyết)</t>
         </is>
       </c>
-      <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
     </row>
     <row r="10" ht="60" customHeight="1">
@@ -1045,7 +1045,7 @@
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>Ngô Văn I</t>
+          <t>Hoàng Thị E</t>
         </is>
       </c>
       <c r="C10" s="7" t="inlineStr"/>
@@ -1056,7 +1056,7 @@
         <is>
           <t>Lớp: CL10
 Môn: Kỹ năng mềm
-Phòng: R104
+Phòng: R101
 (Lý thuyết)</t>
         </is>
       </c>
@@ -1177,21 +1177,21 @@
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>Võ Văn F</t>
+          <t>Hoàng Thị E</t>
         </is>
       </c>
       <c r="C8" s="7" t="inlineStr"/>
-      <c r="D8" s="7" t="inlineStr"/>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL05
+Môn: Kỹ năng mềm
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL10
-Môn: Tiếng Anh chuyên ngành
-Phòng: R102
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
@@ -1204,8 +1204,8 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C1
-(13:00-15:00)</t>
+          <t>C2
+(15:00-17:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -1216,15 +1216,15 @@
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
       <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL05
-Môn: Kỹ năng mềm
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Tiếng Anh chuyên ngành
 Phòng: R103
 (Lý thuyết)</t>
         </is>
       </c>
-      <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
     </row>
     <row r="10" ht="60" customHeight="1">
@@ -1236,7 +1236,7 @@
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>Ngô Văn I</t>
+          <t>Hoàng Thị E</t>
         </is>
       </c>
       <c r="C10" s="7" t="inlineStr"/>
@@ -1247,7 +1247,7 @@
         <is>
           <t>Lớp: CL10
 Môn: Kỹ năng mềm
-Phòng: R104
+Phòng: R101
 (Lý thuyết)</t>
         </is>
       </c>
@@ -1368,21 +1368,21 @@
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>Võ Văn F</t>
+          <t>Hoàng Thị E</t>
         </is>
       </c>
       <c r="C8" s="7" t="inlineStr"/>
-      <c r="D8" s="7" t="inlineStr"/>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL05
+Môn: Kỹ năng mềm
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL10
-Môn: Tiếng Anh chuyên ngành
-Phòng: R102
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
@@ -1395,8 +1395,8 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C1
-(13:00-15:00)</t>
+          <t>C2
+(15:00-17:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -1407,15 +1407,15 @@
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
       <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL05
-Môn: Kỹ năng mềm
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Tiếng Anh chuyên ngành
 Phòng: R103
 (Lý thuyết)</t>
         </is>
       </c>
-      <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
     </row>
     <row r="10" ht="60" customHeight="1">
@@ -1427,7 +1427,7 @@
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>Ngô Văn I</t>
+          <t>Hoàng Thị E</t>
         </is>
       </c>
       <c r="C10" s="7" t="inlineStr"/>
@@ -1438,7 +1438,7 @@
         <is>
           <t>Lớp: CL10
 Môn: Kỹ năng mềm
-Phòng: R104
+Phòng: R101
 (Lý thuyết)</t>
         </is>
       </c>
@@ -1559,21 +1559,21 @@
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>Võ Văn F</t>
+          <t>Hoàng Thị E</t>
         </is>
       </c>
       <c r="C8" s="7" t="inlineStr"/>
-      <c r="D8" s="7" t="inlineStr"/>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL05
+Môn: Kỹ năng mềm
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL10
-Môn: Tiếng Anh chuyên ngành
-Phòng: R102
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
@@ -1586,8 +1586,8 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C1
-(13:00-15:00)</t>
+          <t>C2
+(15:00-17:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -1598,15 +1598,15 @@
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
       <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL05
-Môn: Kỹ năng mềm
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Tiếng Anh chuyên ngành
 Phòng: R103
 (Lý thuyết)</t>
         </is>
       </c>
-      <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
     </row>
     <row r="10" ht="60" customHeight="1">
@@ -1618,7 +1618,7 @@
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>Ngô Văn I</t>
+          <t>Hoàng Thị E</t>
         </is>
       </c>
       <c r="C10" s="7" t="inlineStr"/>
@@ -1629,7 +1629,7 @@
         <is>
           <t>Lớp: CL10
 Môn: Kỹ năng mềm
-Phòng: R104
+Phòng: R101
 (Lý thuyết)</t>
         </is>
       </c>
@@ -1750,21 +1750,21 @@
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>Võ Văn F</t>
+          <t>Hoàng Thị E</t>
         </is>
       </c>
       <c r="C8" s="7" t="inlineStr"/>
-      <c r="D8" s="7" t="inlineStr"/>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL05
+Môn: Kỹ năng mềm
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL10
-Môn: Tiếng Anh chuyên ngành
-Phòng: R102
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
@@ -1777,8 +1777,8 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C1
-(13:00-15:00)</t>
+          <t>C2
+(15:00-17:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -1789,15 +1789,15 @@
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
       <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL05
-Môn: Kỹ năng mềm
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Tiếng Anh chuyên ngành
 Phòng: R103
 (Lý thuyết)</t>
         </is>
       </c>
-      <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
     </row>
     <row r="10" ht="60" customHeight="1">
@@ -1809,7 +1809,7 @@
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>Ngô Văn I</t>
+          <t>Hoàng Thị E</t>
         </is>
       </c>
       <c r="C10" s="7" t="inlineStr"/>
@@ -1820,7 +1820,7 @@
         <is>
           <t>Lớp: CL10
 Môn: Kỹ năng mềm
-Phòng: R104
+Phòng: R101
 (Lý thuyết)</t>
         </is>
       </c>
@@ -1941,21 +1941,21 @@
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>Võ Văn F</t>
+          <t>Hoàng Thị E</t>
         </is>
       </c>
       <c r="C8" s="7" t="inlineStr"/>
-      <c r="D8" s="7" t="inlineStr"/>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL05
+Môn: Kỹ năng mềm
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL10
-Môn: Tiếng Anh chuyên ngành
-Phòng: R102
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
@@ -1968,8 +1968,8 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C1
-(13:00-15:00)</t>
+          <t>C2
+(15:00-17:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -1980,15 +1980,15 @@
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
       <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL05
-Môn: Kỹ năng mềm
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Tiếng Anh chuyên ngành
 Phòng: R103
 (Lý thuyết)</t>
         </is>
       </c>
-      <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
     </row>
     <row r="10" ht="60" customHeight="1">
@@ -2000,7 +2000,7 @@
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>Ngô Văn I</t>
+          <t>Hoàng Thị E</t>
         </is>
       </c>
       <c r="C10" s="7" t="inlineStr"/>
@@ -2011,7 +2011,7 @@
         <is>
           <t>Lớp: CL10
 Môn: Kỹ năng mềm
-Phòng: R104
+Phòng: R101
 (Lý thuyết)</t>
         </is>
       </c>
@@ -2132,21 +2132,21 @@
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>Võ Văn F</t>
+          <t>Hoàng Thị E</t>
         </is>
       </c>
       <c r="C8" s="7" t="inlineStr"/>
-      <c r="D8" s="7" t="inlineStr"/>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL05
+Môn: Kỹ năng mềm
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL10
-Môn: Tiếng Anh chuyên ngành
-Phòng: R102
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
@@ -2159,8 +2159,8 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C1
-(13:00-15:00)</t>
+          <t>C2
+(15:00-17:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -2171,15 +2171,15 @@
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
       <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL05
-Môn: Kỹ năng mềm
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Tiếng Anh chuyên ngành
 Phòng: R103
 (Lý thuyết)</t>
         </is>
       </c>
-      <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
     </row>
     <row r="10" ht="60" customHeight="1">
@@ -2191,7 +2191,7 @@
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>Ngô Văn I</t>
+          <t>Hoàng Thị E</t>
         </is>
       </c>
       <c r="C10" s="7" t="inlineStr"/>
@@ -2202,7 +2202,7 @@
         <is>
           <t>Lớp: CL10
 Môn: Kỹ năng mềm
-Phòng: R104
+Phòng: R101
 (Lý thuyết)</t>
         </is>
       </c>
@@ -2323,21 +2323,21 @@
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>Võ Văn F</t>
+          <t>Hoàng Thị E</t>
         </is>
       </c>
       <c r="C8" s="7" t="inlineStr"/>
-      <c r="D8" s="7" t="inlineStr"/>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL05
+Môn: Kỹ năng mềm
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL10
-Môn: Tiếng Anh chuyên ngành
-Phòng: R102
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
@@ -2350,8 +2350,8 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C1
-(13:00-15:00)</t>
+          <t>C2
+(15:00-17:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -2362,15 +2362,15 @@
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
       <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL05
-Môn: Kỹ năng mềm
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Tiếng Anh chuyên ngành
 Phòng: R103
 (Lý thuyết)</t>
         </is>
       </c>
-      <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
     </row>
     <row r="10" ht="60" customHeight="1">
@@ -2382,7 +2382,7 @@
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>Ngô Văn I</t>
+          <t>Hoàng Thị E</t>
         </is>
       </c>
       <c r="C10" s="7" t="inlineStr"/>
@@ -2393,7 +2393,7 @@
         <is>
           <t>Lớp: CL10
 Môn: Kỹ năng mềm
-Phòng: R104
+Phòng: R101
 (Lý thuyết)</t>
         </is>
       </c>
@@ -2514,21 +2514,21 @@
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>Võ Văn F</t>
+          <t>Hoàng Thị E</t>
         </is>
       </c>
       <c r="C8" s="7" t="inlineStr"/>
-      <c r="D8" s="7" t="inlineStr"/>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL05
+Môn: Kỹ năng mềm
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL10
-Môn: Tiếng Anh chuyên ngành
-Phòng: R102
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
@@ -2541,8 +2541,8 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C1
-(13:00-15:00)</t>
+          <t>C2
+(15:00-17:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -2553,15 +2553,15 @@
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
       <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL05
-Môn: Kỹ năng mềm
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Tiếng Anh chuyên ngành
 Phòng: R103
 (Lý thuyết)</t>
         </is>
       </c>
-      <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
     </row>
     <row r="10" ht="60" customHeight="1">
@@ -2573,7 +2573,7 @@
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>Ngô Văn I</t>
+          <t>Hoàng Thị E</t>
         </is>
       </c>
       <c r="C10" s="7" t="inlineStr"/>
@@ -2584,7 +2584,7 @@
         <is>
           <t>Lớp: CL10
 Môn: Kỹ năng mềm
-Phòng: R104
+Phòng: R101
 (Lý thuyết)</t>
         </is>
       </c>
@@ -2705,21 +2705,21 @@
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>Võ Văn F</t>
+          <t>Hoàng Thị E</t>
         </is>
       </c>
       <c r="C8" s="7" t="inlineStr"/>
-      <c r="D8" s="7" t="inlineStr"/>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL05
+Môn: Kỹ năng mềm
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL10
-Môn: Tiếng Anh chuyên ngành
-Phòng: R102
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
@@ -2732,8 +2732,8 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C1
-(13:00-15:00)</t>
+          <t>C2
+(15:00-17:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -2744,15 +2744,15 @@
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
       <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL05
-Môn: Kỹ năng mềm
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Tiếng Anh chuyên ngành
 Phòng: R103
 (Lý thuyết)</t>
         </is>
       </c>
-      <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
     </row>
     <row r="10" ht="60" customHeight="1">
@@ -2764,7 +2764,7 @@
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>Ngô Văn I</t>
+          <t>Hoàng Thị E</t>
         </is>
       </c>
       <c r="C10" s="7" t="inlineStr"/>
@@ -2775,7 +2775,7 @@
         <is>
           <t>Lớp: CL10
 Môn: Kỹ năng mềm
-Phòng: R104
+Phòng: R101
 (Lý thuyết)</t>
         </is>
       </c>
@@ -2896,21 +2896,21 @@
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>Võ Văn F</t>
+          <t>Hoàng Thị E</t>
         </is>
       </c>
       <c r="C8" s="7" t="inlineStr"/>
-      <c r="D8" s="7" t="inlineStr"/>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL05
+Môn: Kỹ năng mềm
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL10
-Môn: Tiếng Anh chuyên ngành
-Phòng: R102
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
@@ -2923,8 +2923,8 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C1
-(13:00-15:00)</t>
+          <t>C2
+(15:00-17:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -2935,15 +2935,15 @@
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
       <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL05
-Môn: Kỹ năng mềm
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Tiếng Anh chuyên ngành
 Phòng: R103
 (Lý thuyết)</t>
         </is>
       </c>
-      <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
     </row>
     <row r="10" ht="60" customHeight="1">
@@ -2955,7 +2955,7 @@
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>Ngô Văn I</t>
+          <t>Hoàng Thị E</t>
         </is>
       </c>
       <c r="C10" s="7" t="inlineStr"/>
@@ -2966,7 +2966,7 @@
         <is>
           <t>Lớp: CL10
 Môn: Kỹ năng mềm
-Phòng: R104
+Phòng: R101
 (Lý thuyết)</t>
         </is>
       </c>
@@ -3087,21 +3087,21 @@
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>Võ Văn F</t>
+          <t>Hoàng Thị E</t>
         </is>
       </c>
       <c r="C8" s="7" t="inlineStr"/>
-      <c r="D8" s="7" t="inlineStr"/>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL05
+Môn: Kỹ năng mềm
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL10
-Môn: Tiếng Anh chuyên ngành
-Phòng: R102
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
@@ -3114,8 +3114,8 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C1
-(13:00-15:00)</t>
+          <t>C2
+(15:00-17:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -3126,15 +3126,15 @@
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
       <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL05
-Môn: Kỹ năng mềm
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Tiếng Anh chuyên ngành
 Phòng: R103
 (Lý thuyết)</t>
         </is>
       </c>
-      <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
     </row>
     <row r="10" ht="60" customHeight="1">
@@ -3146,7 +3146,7 @@
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>Ngô Văn I</t>
+          <t>Hoàng Thị E</t>
         </is>
       </c>
       <c r="C10" s="7" t="inlineStr"/>
@@ -3157,7 +3157,7 @@
         <is>
           <t>Lớp: CL10
 Môn: Kỹ năng mềm
-Phòng: R104
+Phòng: R101
 (Lý thuyết)</t>
         </is>
       </c>
@@ -3278,21 +3278,21 @@
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>Võ Văn F</t>
+          <t>Hoàng Thị E</t>
         </is>
       </c>
       <c r="C8" s="7" t="inlineStr"/>
-      <c r="D8" s="7" t="inlineStr"/>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL05
+Môn: Kỹ năng mềm
+Phòng: R103
+(Lý thuyết)</t>
+        </is>
+      </c>
       <c r="E8" s="7" t="inlineStr"/>
       <c r="F8" s="7" t="inlineStr"/>
-      <c r="G8" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL10
-Môn: Tiếng Anh chuyên ngành
-Phòng: R102
-(Lý thuyết)</t>
-        </is>
-      </c>
+      <c r="G8" s="7" t="inlineStr"/>
       <c r="H8" s="8" t="inlineStr">
         <is>
           <t>Lớp: CL05
@@ -3305,8 +3305,8 @@
     <row r="9" ht="60" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>C1
-(13:00-15:00)</t>
+          <t>C2
+(15:00-17:00)</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
@@ -3317,15 +3317,15 @@
       <c r="C9" s="7" t="inlineStr"/>
       <c r="D9" s="7" t="inlineStr"/>
       <c r="E9" s="7" t="inlineStr"/>
-      <c r="F9" s="8" t="inlineStr">
-        <is>
-          <t>Lớp: CL05
-Môn: Kỹ năng mềm
+      <c r="F9" s="7" t="inlineStr"/>
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>Lớp: CL10
+Môn: Tiếng Anh chuyên ngành
 Phòng: R103
 (Lý thuyết)</t>
         </is>
       </c>
-      <c r="G9" s="7" t="inlineStr"/>
       <c r="H9" s="7" t="inlineStr"/>
     </row>
     <row r="10" ht="60" customHeight="1">
@@ -3337,7 +3337,7 @@
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>Ngô Văn I</t>
+          <t>Hoàng Thị E</t>
         </is>
       </c>
       <c r="C10" s="7" t="inlineStr"/>
@@ -3348,7 +3348,7 @@
         <is>
           <t>Lớp: CL10
 Môn: Kỹ năng mềm
-Phòng: R104
+Phòng: R101
 (Lý thuyết)</t>
         </is>
       </c>

</xml_diff>